<commit_message>
update monitoring week 1 dan 2
</commit_message>
<xml_diff>
--- a/RichieChristiansenSenlia/Richie.xlsx
+++ b/RichieChristiansenSenlia/Richie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ontologi-Sejarah-Indonesia\RichieChristiansenSenlia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F65648-0692-429E-A1F0-0AC00F67AEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9C132D-3BC9-491C-B522-610D9F667A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="128">
   <si>
     <t>Monitoring Skripsi dari:</t>
   </si>
@@ -477,6 +477,23 @@
 2. mengidentifikasi jenis infobox yang didapatkan
 3. membersihkan data pada infobox
 4. melakukan mapping infobox ke rdf</t>
+  </si>
+  <si>
+    <t>Alokasi waktu: 12 jam 
+Link Commit: ....
+Uraian: Melakukan filtering artikel artikel yang didapat dari idwikidump berdasarkan kategori sejarah nusantara dan mengekstrak infobox dari artikel artikel tersebut</t>
+  </si>
+  <si>
+    <t>1. Menelusuri artikel wikipedia berdasarkan templat - templat yang relevan</t>
+  </si>
+  <si>
+    <t>Alokasi waktu: 15 jam 
+Link Commit: ....
+Uraian: Melakukan eksplorasi sejarah kolonialisme Indonesia berdasarkan sejarah nasional indonesia jilid 4 dan mendaftar entitas entitas yang ditemukan. Entitas tersebut kemudian dicari keberadaan data pada dbpedia dan juga sumber data lainnya seperti anri dan britannica.com</t>
+  </si>
+  <si>
+    <t>1. eksplorasi data wikidump
+2. memfilter artikel wikipedia berdasarkan kategori</t>
   </si>
 </sst>
 </file>
@@ -1072,10 +1089,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1084,12 +1107,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1368,7 +1385,7 @@
   <dimension ref="A1:AE1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
       <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
@@ -1390,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="97" t="s">
         <v>121</v>
       </c>
       <c r="D1" s="95"/>
@@ -1422,7 +1439,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="96" t="s">
+      <c r="C2" s="98" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="95"/>
@@ -1581,7 +1598,7 @@
       <c r="B7" s="4"/>
       <c r="C7" s="15"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="97"/>
+      <c r="E7" s="99"/>
       <c r="F7" s="95"/>
       <c r="G7" s="95"/>
       <c r="H7" s="95"/>
@@ -1971,10 +1988,10 @@
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="23" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="H14" s="23" t="s">
         <v>122</v>
@@ -2037,8 +2054,12 @@
       <c r="C15" s="17"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
+      <c r="F15" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>125</v>
+      </c>
       <c r="H15" s="23" t="s">
         <v>123</v>
       </c>
@@ -2244,7 +2265,7 @@
       <c r="AE19" s="4"/>
     </row>
     <row r="20" spans="1:31" ht="13" x14ac:dyDescent="0.25">
-      <c r="A20" s="98" t="s">
+      <c r="A20" s="100" t="s">
         <v>40</v>
       </c>
       <c r="B20" s="95"/>
@@ -2593,7 +2614,7 @@
       <c r="AE24" s="4"/>
     </row>
     <row r="25" spans="1:31" ht="13" x14ac:dyDescent="0.25">
-      <c r="A25" s="98" t="s">
+      <c r="A25" s="100" t="s">
         <v>45</v>
       </c>
       <c r="B25" s="95"/>
@@ -2761,7 +2782,7 @@
       <c r="AE28" s="4"/>
     </row>
     <row r="29" spans="1:31" ht="13" x14ac:dyDescent="0.25">
-      <c r="A29" s="99" t="s">
+      <c r="A29" s="94" t="s">
         <v>52</v>
       </c>
       <c r="B29" s="95"/>
@@ -4595,7 +4616,7 @@
       <c r="AE52" s="4"/>
     </row>
     <row r="53" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="100" t="s">
+      <c r="A53" s="96" t="s">
         <v>76</v>
       </c>
       <c r="B53" s="95"/>
@@ -36047,12 +36068,12 @@
     <col min="3" max="3" width="62.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="70"/>
       <c r="B1" s="70"/>
       <c r="C1" s="42"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="70"/>
       <c r="B2" s="71">
         <f>COUNTIF(B3:B15,TRUE())/13</f>
@@ -40092,12 +40113,12 @@
     <col min="3" max="3" width="62.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="70"/>
       <c r="B1" s="70"/>
       <c r="C1" s="42"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="70"/>
       <c r="B2" s="78">
         <f>COUNTIF(B3:B13,TRUE())/11</f>
@@ -44120,7 +44141,7 @@
     <col min="5" max="5" width="26.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="85" t="s">
         <v>115</v>
       </c>

</xml_diff>